<commit_message>
a minor data table structure change
Move CoopNodeID and PickNodeID columns from LineItem table to Skus Table
</commit_message>
<xml_diff>
--- a/PickerTransporterCooperation/Order_Skus.xlsx
+++ b/PickerTransporterCooperation/Order_Skus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/jzl0196_auburn_edu/Documents/Doctor work/Summer2020/coop-temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/jzl0196_auburn_edu/Documents/Doctor work/Summer2020/Github/SimioExampleModels/PickerTransporterCooperation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="11_AD4DA82427541F7ACA7EB8BC18CA0F0A6BE8DE10" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32CC873B-A71B-45B9-A337-B8D33C2C1CAF}"/>
+  <xr:revisionPtr revIDLastSave="322" documentId="11_AD4DA82427541F7ACA7EB8BC18CA0F0A6BE8DE10" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7623200-05CA-4234-90E6-7EA2AF798B52}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="2715" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>OrderID</t>
   </si>
@@ -67,12 +67,15 @@
   <si>
     <t>TransporterID</t>
   </si>
+  <si>
+    <t>BatchID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +85,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,10 +115,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,9 +127,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +450,7 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -481,18 +497,108 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="2"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B046AA82-2A84-4475-8A7B-E81811DBFE57}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -539,10 +645,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9EE495-3BE9-46CD-B425-BEFC319920F6}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +656,7 @@
     <col min="1" max="16384" width="18.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,8 +684,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -607,8 +716,11 @@
       <c r="I2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -636,8 +748,11 @@
       <c r="I3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -665,8 +780,11 @@
       <c r="I4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -694,8 +812,11 @@
       <c r="I5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -723,8 +844,11 @@
       <c r="I6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -752,8 +876,11 @@
       <c r="I7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -779,6 +906,425 @@
         <v>3</v>
       </c>
       <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>19</v>
+      </c>
+      <c r="E21" s="1">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3</v>
+      </c>
+      <c r="J21" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a new example
Add a new example about multiple vehicle use the same table for different fixed routes.
</commit_message>
<xml_diff>
--- a/PickerTransporterCooperation/Order_Skus.xlsx
+++ b/PickerTransporterCooperation/Order_Skus.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/jzl0196_auburn_edu/Documents/Doctor work/Summer2020/Github/SimioExampleModels/PickerTransporterCooperation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="114_{B8E9BF05-B438-4067-9704-1816358A597D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9FC3895-9DAD-4E85-8D3A-8B42034B0BB5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="8145" yWindow="2610" windowWidth="38700" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
     <sheet name="Skus" sheetId="2" r:id="rId2"/>
     <sheet name="LineItem" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -75,11 +81,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -189,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +235,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,6 +287,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,14 +480,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -462,7 +512,7 @@
         <v>43960</v>
       </c>
       <c r="C2" s="2">
-        <v>43963.99998842592</v>
+        <v>43963.999988425923</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -471,7 +521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -479,7 +529,7 @@
         <v>43960</v>
       </c>
       <c r="C3" s="2">
-        <v>43965.99998842592</v>
+        <v>43965.999988425923</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -488,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -496,7 +546,7 @@
         <v>43960</v>
       </c>
       <c r="C4" s="2">
-        <v>43966.99998842592</v>
+        <v>43966.999988425923</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -505,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -513,7 +563,7 @@
         <v>43960</v>
       </c>
       <c r="C5" s="2">
-        <v>43966.99998842592</v>
+        <v>43966.999988425923</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -522,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -530,7 +580,7 @@
         <v>43960</v>
       </c>
       <c r="C6" s="2">
-        <v>43969.99998842592</v>
+        <v>43969.999988425923</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -539,7 +589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -547,7 +597,7 @@
         <v>43960</v>
       </c>
       <c r="C7" s="2">
-        <v>43970.99998842592</v>
+        <v>43970.999988425923</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -556,7 +606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -564,7 +614,7 @@
         <v>43960</v>
       </c>
       <c r="C8" s="2">
-        <v>43970.99998842592</v>
+        <v>43970.999988425923</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -573,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -581,7 +631,7 @@
         <v>43960</v>
       </c>
       <c r="C9" s="2">
-        <v>43970.99998842592</v>
+        <v>43970.999988425923</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -590,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -598,7 +648,7 @@
         <v>43960</v>
       </c>
       <c r="C10" s="2">
-        <v>43971.99998842592</v>
+        <v>43971.999988425923</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -607,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -615,7 +665,7 @@
         <v>43960</v>
       </c>
       <c r="C11" s="2">
-        <v>43972.99998842592</v>
+        <v>43972.999988425923</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -630,14 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -659,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -670,7 +720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -681,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -692,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -703,7 +753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -714,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -725,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -736,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -747,7 +797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -764,14 +814,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="35.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -841,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -876,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -911,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -946,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -981,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1016,7 +1071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1051,7 +1106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1086,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1121,7 +1176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1156,7 +1211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1191,7 +1246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1226,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1261,7 +1316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1296,7 +1351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1331,7 +1386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1366,7 +1421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1401,7 +1456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1436,7 +1491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1471,7 +1526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1506,7 +1561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1541,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1576,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1611,7 +1666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1646,7 +1701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1681,7 +1736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1716,7 +1771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1751,7 +1806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1786,7 +1841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1821,7 +1876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1856,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1891,7 +1946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
@@ -1926,7 +1981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
@@ -1961,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1996,7 +2051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -2031,7 +2086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -2066,7 +2121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2101,7 +2156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2136,7 +2191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2171,7 +2226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2206,7 +2261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2241,7 +2296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2276,7 +2331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2311,7 +2366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2346,7 +2401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
@@ -2381,7 +2436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2416,7 +2471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2451,7 +2506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2486,7 +2541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6</v>
       </c>
@@ -2521,7 +2576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2556,7 +2611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7</v>
       </c>
@@ -2591,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>8</v>
       </c>
@@ -2626,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9</v>
       </c>
@@ -2661,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>10</v>
       </c>
@@ -2696,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9</v>
       </c>
@@ -2731,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>8</v>
       </c>
@@ -2766,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9</v>
       </c>
@@ -2801,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -2836,7 +2891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9</v>
       </c>
@@ -2871,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8</v>
       </c>
@@ -2906,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
@@ -2941,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>8</v>
       </c>
@@ -2976,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9</v>
       </c>
@@ -3011,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>10</v>
       </c>
@@ -3046,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7</v>
       </c>
@@ -3081,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3116,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>8</v>
       </c>
@@ -3151,7 +3206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>8</v>
       </c>
@@ -3186,7 +3241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9</v>
       </c>
@@ -3221,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9</v>
       </c>
@@ -3256,7 +3311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>8</v>
       </c>
@@ -3291,7 +3346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>8</v>
       </c>
@@ -3326,7 +3381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7</v>
       </c>
@@ -3361,7 +3416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>10</v>
       </c>
@@ -3396,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>7</v>
       </c>
@@ -3431,7 +3486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3466,7 +3521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>7</v>
       </c>
@@ -3501,7 +3556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>10</v>
       </c>
@@ -3536,7 +3591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>7</v>
       </c>
@@ -3571,7 +3626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>10</v>
       </c>
@@ -3606,7 +3661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>10</v>
       </c>

</xml_diff>